<commit_message>
Revision de no conformidades
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1346 - AECCON, Rigoberto Orozco_OC/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/11/P1346 - AECCON, Rigoberto Orozco_OC/Calidad/No_conformidades.xlsx
@@ -47,7 +47,7 @@
     <t>Oriana Osiris</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
   </si>
   <si>
     <t>Agregar fecha real de cierre en el hito de cierre</t>
@@ -295,7 +295,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>